<commit_message>
walk through all steps
</commit_message>
<xml_diff>
--- a/synthetic_data_generating/one_to_one/data_2.xlsx
+++ b/synthetic_data_generating/one_to_one/data_2.xlsx
@@ -8,19 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caijunjie/Documents/learning/IIT_Master/CS584/synthetic_data_generating/synthetic_data_generating/one_to_one/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E50902BD-1D38-064A-B02A-55C006F6BA19}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87CF7679-A3C4-B643-BD1B-F6E04920AEF6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="19560" windowHeight="15420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$101</definedName>
+  </definedNames>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>id</t>
   </si>
@@ -29,24 +32,6 @@
   </si>
   <si>
     <t>d</t>
-  </si>
-  <si>
-    <t>c1</t>
-  </si>
-  <si>
-    <t>c2</t>
-  </si>
-  <si>
-    <t>c3</t>
-  </si>
-  <si>
-    <t>d3</t>
-  </si>
-  <si>
-    <t>d2</t>
-  </si>
-  <si>
-    <t>d1</t>
   </si>
 </sst>
 </file>
@@ -105,11 +90,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,19 +440,22 @@
   <dimension ref="A1:C101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="3" width="8.83203125" style="3"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
@@ -471,1103 +463,1104 @@
       <c r="A2">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
+      <c r="B2" s="3">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="B3" s="3">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
+      <c r="B4" s="3">
+        <v>2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
+      <c r="B5" s="3">
+        <v>2</v>
+      </c>
+      <c r="C5" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
+      <c r="B6" s="3">
+        <v>2</v>
+      </c>
+      <c r="C6" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
+      <c r="B7" s="3">
+        <v>3</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
+      <c r="B8" s="3">
+        <v>2</v>
+      </c>
+      <c r="C8" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
+      <c r="B9" s="3">
+        <v>1</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>4</v>
-      </c>
-      <c r="C10" t="s">
-        <v>8</v>
+      <c r="B10" s="3">
+        <v>2</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>9</v>
       </c>
-      <c r="B11" t="s">
-        <v>3</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
+      <c r="B11" s="3">
+        <v>1</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>4</v>
-      </c>
-      <c r="C12" t="s">
-        <v>8</v>
+      <c r="B12" s="3">
+        <v>2</v>
+      </c>
+      <c r="C12" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>11</v>
       </c>
-      <c r="B13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" t="s">
-        <v>6</v>
+      <c r="B13" s="3">
+        <v>3</v>
+      </c>
+      <c r="C13" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>12</v>
       </c>
-      <c r="B14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
+      <c r="B14" s="3">
+        <v>1</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>13</v>
       </c>
-      <c r="B15" t="s">
-        <v>4</v>
-      </c>
-      <c r="C15" t="s">
-        <v>8</v>
+      <c r="B15" s="3">
+        <v>2</v>
+      </c>
+      <c r="C15" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>14</v>
       </c>
-      <c r="B16" t="s">
-        <v>3</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
+      <c r="B16" s="3">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>15</v>
       </c>
-      <c r="B17" t="s">
-        <v>5</v>
-      </c>
-      <c r="C17" t="s">
-        <v>8</v>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>16</v>
       </c>
-      <c r="B18" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
+      <c r="B18" s="3">
+        <v>2</v>
+      </c>
+      <c r="C18" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>17</v>
       </c>
-      <c r="B19" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" t="s">
-        <v>8</v>
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>18</v>
       </c>
-      <c r="B20" t="s">
-        <v>5</v>
-      </c>
-      <c r="C20" t="s">
-        <v>7</v>
+      <c r="B20" s="3">
+        <v>3</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>19</v>
       </c>
-      <c r="B21" t="s">
-        <v>4</v>
-      </c>
-      <c r="C21" t="s">
-        <v>7</v>
+      <c r="B21" s="3">
+        <v>2</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>20</v>
       </c>
-      <c r="B22" t="s">
-        <v>3</v>
-      </c>
-      <c r="C22" t="s">
-        <v>8</v>
+      <c r="B22" s="3">
+        <v>1</v>
+      </c>
+      <c r="C22" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>21</v>
       </c>
-      <c r="B23" t="s">
-        <v>5</v>
-      </c>
-      <c r="C23" t="s">
-        <v>8</v>
+      <c r="B23" s="3">
+        <v>3</v>
+      </c>
+      <c r="C23" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>22</v>
       </c>
-      <c r="B24" t="s">
-        <v>4</v>
-      </c>
-      <c r="C24" t="s">
-        <v>7</v>
+      <c r="B24" s="3">
+        <v>2</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>23</v>
       </c>
-      <c r="B25" t="s">
-        <v>4</v>
-      </c>
-      <c r="C25" t="s">
-        <v>8</v>
+      <c r="B25" s="3">
+        <v>2</v>
+      </c>
+      <c r="C25" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>24</v>
       </c>
-      <c r="B26" t="s">
-        <v>5</v>
-      </c>
-      <c r="C26" t="s">
-        <v>6</v>
+      <c r="B26" s="3">
+        <v>3</v>
+      </c>
+      <c r="C26" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>25</v>
       </c>
-      <c r="B27" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
+      <c r="B27" s="3">
+        <v>1</v>
+      </c>
+      <c r="C27" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>4</v>
-      </c>
-      <c r="C28" t="s">
-        <v>8</v>
+      <c r="B28" s="3">
+        <v>2</v>
+      </c>
+      <c r="C28" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>27</v>
       </c>
-      <c r="B29" t="s">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>8</v>
+      <c r="B29" s="3">
+        <v>1</v>
+      </c>
+      <c r="C29" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>28</v>
       </c>
-      <c r="B30" t="s">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
+      <c r="B30" s="3">
+        <v>2</v>
+      </c>
+      <c r="C30" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>29</v>
       </c>
-      <c r="B31" t="s">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>8</v>
+      <c r="B31" s="3">
+        <v>3</v>
+      </c>
+      <c r="C31" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>30</v>
       </c>
-      <c r="B32" t="s">
-        <v>5</v>
-      </c>
-      <c r="C32" t="s">
-        <v>6</v>
+      <c r="B32" s="3">
+        <v>3</v>
+      </c>
+      <c r="C32" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>31</v>
       </c>
-      <c r="B33" t="s">
-        <v>3</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
+      <c r="B33" s="3">
+        <v>1</v>
+      </c>
+      <c r="C33" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>32</v>
       </c>
-      <c r="B34" t="s">
-        <v>4</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
+      <c r="B34" s="3">
+        <v>2</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>33</v>
       </c>
-      <c r="B35" t="s">
-        <v>5</v>
-      </c>
-      <c r="C35" t="s">
-        <v>6</v>
+      <c r="B35" s="3">
+        <v>3</v>
+      </c>
+      <c r="C35" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>34</v>
       </c>
-      <c r="B36" t="s">
-        <v>3</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
+      <c r="B36" s="3">
+        <v>1</v>
+      </c>
+      <c r="C36" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>35</v>
       </c>
-      <c r="B37" t="s">
-        <v>3</v>
-      </c>
-      <c r="C37" t="s">
-        <v>8</v>
+      <c r="B37" s="3">
+        <v>1</v>
+      </c>
+      <c r="C37" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>36</v>
       </c>
-      <c r="B38" t="s">
-        <v>5</v>
-      </c>
-      <c r="C38" t="s">
-        <v>8</v>
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>37</v>
       </c>
-      <c r="B39" t="s">
-        <v>5</v>
-      </c>
-      <c r="C39" t="s">
-        <v>7</v>
+      <c r="B39" s="3">
+        <v>3</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>38</v>
       </c>
-      <c r="B40" t="s">
-        <v>4</v>
-      </c>
-      <c r="C40" t="s">
-        <v>8</v>
+      <c r="B40" s="3">
+        <v>2</v>
+      </c>
+      <c r="C40" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>39</v>
       </c>
-      <c r="B41" t="s">
-        <v>4</v>
-      </c>
-      <c r="C41" t="s">
-        <v>6</v>
+      <c r="B41" s="3">
+        <v>2</v>
+      </c>
+      <c r="C41" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>40</v>
       </c>
-      <c r="B42" t="s">
-        <v>5</v>
-      </c>
-      <c r="C42" t="s">
-        <v>7</v>
+      <c r="B42" s="3">
+        <v>3</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A43">
         <v>41</v>
       </c>
-      <c r="B43" t="s">
-        <v>5</v>
-      </c>
-      <c r="C43" t="s">
-        <v>7</v>
+      <c r="B43" s="3">
+        <v>3</v>
+      </c>
+      <c r="C43" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A44">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>7</v>
+      <c r="B44" s="3">
+        <v>3</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45">
         <v>43</v>
       </c>
-      <c r="B45" t="s">
-        <v>4</v>
-      </c>
-      <c r="C45" t="s">
-        <v>6</v>
+      <c r="B45" s="3">
+        <v>2</v>
+      </c>
+      <c r="C45" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46">
         <v>44</v>
       </c>
-      <c r="B46" t="s">
-        <v>4</v>
-      </c>
-      <c r="C46" t="s">
-        <v>6</v>
+      <c r="B46" s="3">
+        <v>2</v>
+      </c>
+      <c r="C46" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A47">
         <v>45</v>
       </c>
-      <c r="B47" t="s">
-        <v>4</v>
-      </c>
-      <c r="C47" t="s">
-        <v>6</v>
+      <c r="B47" s="3">
+        <v>2</v>
+      </c>
+      <c r="C47" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A48">
         <v>46</v>
       </c>
-      <c r="B48" t="s">
-        <v>3</v>
-      </c>
-      <c r="C48" t="s">
-        <v>6</v>
+      <c r="B48" s="3">
+        <v>1</v>
+      </c>
+      <c r="C48" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49">
         <v>47</v>
       </c>
-      <c r="B49" t="s">
-        <v>3</v>
-      </c>
-      <c r="C49" t="s">
-        <v>7</v>
+      <c r="B49" s="3">
+        <v>1</v>
+      </c>
+      <c r="C49" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A50">
         <v>48</v>
       </c>
-      <c r="B50" t="s">
-        <v>3</v>
-      </c>
-      <c r="C50" t="s">
-        <v>6</v>
+      <c r="B50" s="3">
+        <v>1</v>
+      </c>
+      <c r="C50" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A51">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
-        <v>5</v>
-      </c>
-      <c r="C51" t="s">
-        <v>8</v>
+      <c r="B51" s="3">
+        <v>3</v>
+      </c>
+      <c r="C51" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A52">
         <v>50</v>
       </c>
-      <c r="B52" t="s">
-        <v>5</v>
-      </c>
-      <c r="C52" t="s">
-        <v>8</v>
+      <c r="B52" s="3">
+        <v>3</v>
+      </c>
+      <c r="C52" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A53">
         <v>51</v>
       </c>
-      <c r="B53" t="s">
-        <v>4</v>
-      </c>
-      <c r="C53" t="s">
-        <v>7</v>
+      <c r="B53" s="3">
+        <v>2</v>
+      </c>
+      <c r="C53" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A54">
         <v>52</v>
       </c>
-      <c r="B54" t="s">
-        <v>4</v>
-      </c>
-      <c r="C54" t="s">
-        <v>6</v>
+      <c r="B54" s="3">
+        <v>2</v>
+      </c>
+      <c r="C54" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A55">
         <v>53</v>
       </c>
-      <c r="B55" t="s">
-        <v>4</v>
-      </c>
-      <c r="C55" t="s">
-        <v>6</v>
+      <c r="B55" s="3">
+        <v>2</v>
+      </c>
+      <c r="C55" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A56">
         <v>54</v>
       </c>
-      <c r="B56" t="s">
-        <v>3</v>
-      </c>
-      <c r="C56" t="s">
-        <v>8</v>
+      <c r="B56" s="3">
+        <v>1</v>
+      </c>
+      <c r="C56" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A57">
         <v>55</v>
       </c>
-      <c r="B57" t="s">
-        <v>5</v>
-      </c>
-      <c r="C57" t="s">
-        <v>7</v>
+      <c r="B57" s="3">
+        <v>3</v>
+      </c>
+      <c r="C57" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A58">
         <v>56</v>
       </c>
-      <c r="B58" t="s">
-        <v>5</v>
-      </c>
-      <c r="C58" t="s">
-        <v>8</v>
+      <c r="B58" s="3">
+        <v>3</v>
+      </c>
+      <c r="C58" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A59">
         <v>57</v>
       </c>
-      <c r="B59" t="s">
-        <v>5</v>
-      </c>
-      <c r="C59" t="s">
-        <v>8</v>
+      <c r="B59" s="3">
+        <v>3</v>
+      </c>
+      <c r="C59" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A60">
         <v>58</v>
       </c>
-      <c r="B60" t="s">
-        <v>5</v>
-      </c>
-      <c r="C60" t="s">
-        <v>6</v>
+      <c r="B60" s="3">
+        <v>3</v>
+      </c>
+      <c r="C60" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A61">
         <v>59</v>
       </c>
-      <c r="B61" t="s">
-        <v>4</v>
-      </c>
-      <c r="C61" t="s">
-        <v>8</v>
+      <c r="B61" s="3">
+        <v>2</v>
+      </c>
+      <c r="C61" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A62">
         <v>60</v>
       </c>
-      <c r="B62" t="s">
-        <v>3</v>
-      </c>
-      <c r="C62" t="s">
-        <v>8</v>
+      <c r="B62" s="3">
+        <v>1</v>
+      </c>
+      <c r="C62" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A63">
         <v>61</v>
       </c>
-      <c r="B63" t="s">
-        <v>4</v>
-      </c>
-      <c r="C63" t="s">
-        <v>7</v>
+      <c r="B63" s="3">
+        <v>2</v>
+      </c>
+      <c r="C63" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A64">
         <v>62</v>
       </c>
-      <c r="B64" t="s">
-        <v>4</v>
-      </c>
-      <c r="C64" t="s">
-        <v>8</v>
+      <c r="B64" s="3">
+        <v>2</v>
+      </c>
+      <c r="C64" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A65">
         <v>63</v>
       </c>
-      <c r="B65" t="s">
-        <v>5</v>
-      </c>
-      <c r="C65" t="s">
-        <v>7</v>
+      <c r="B65" s="3">
+        <v>3</v>
+      </c>
+      <c r="C65" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66">
         <v>64</v>
       </c>
-      <c r="B66" t="s">
-        <v>4</v>
-      </c>
-      <c r="C66" t="s">
-        <v>7</v>
+      <c r="B66" s="3">
+        <v>2</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A67">
         <v>65</v>
       </c>
-      <c r="B67" t="s">
-        <v>3</v>
-      </c>
-      <c r="C67" t="s">
-        <v>7</v>
+      <c r="B67" s="3">
+        <v>1</v>
+      </c>
+      <c r="C67" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68">
         <v>66</v>
       </c>
-      <c r="B68" t="s">
-        <v>4</v>
-      </c>
-      <c r="C68" t="s">
-        <v>6</v>
+      <c r="B68" s="3">
+        <v>2</v>
+      </c>
+      <c r="C68" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69">
         <v>67</v>
       </c>
-      <c r="B69" t="s">
-        <v>4</v>
-      </c>
-      <c r="C69" t="s">
-        <v>8</v>
+      <c r="B69" s="3">
+        <v>2</v>
+      </c>
+      <c r="C69" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A70">
         <v>68</v>
       </c>
-      <c r="B70" t="s">
-        <v>5</v>
-      </c>
-      <c r="C70" t="s">
-        <v>6</v>
+      <c r="B70" s="3">
+        <v>3</v>
+      </c>
+      <c r="C70" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A71">
         <v>69</v>
       </c>
-      <c r="B71" t="s">
-        <v>3</v>
-      </c>
-      <c r="C71" t="s">
-        <v>7</v>
+      <c r="B71" s="3">
+        <v>1</v>
+      </c>
+      <c r="C71" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A72">
         <v>70</v>
       </c>
-      <c r="B72" t="s">
-        <v>4</v>
-      </c>
-      <c r="C72" t="s">
-        <v>8</v>
+      <c r="B72" s="3">
+        <v>2</v>
+      </c>
+      <c r="C72" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A73">
         <v>71</v>
       </c>
-      <c r="B73" t="s">
-        <v>5</v>
-      </c>
-      <c r="C73" t="s">
-        <v>7</v>
+      <c r="B73" s="3">
+        <v>3</v>
+      </c>
+      <c r="C73" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A74">
         <v>72</v>
       </c>
-      <c r="B74" t="s">
-        <v>4</v>
-      </c>
-      <c r="C74" t="s">
-        <v>7</v>
+      <c r="B74" s="3">
+        <v>2</v>
+      </c>
+      <c r="C74" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A75">
         <v>73</v>
       </c>
-      <c r="B75" t="s">
-        <v>4</v>
-      </c>
-      <c r="C75" t="s">
-        <v>8</v>
+      <c r="B75" s="3">
+        <v>2</v>
+      </c>
+      <c r="C75" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A76">
         <v>74</v>
       </c>
-      <c r="B76" t="s">
-        <v>4</v>
-      </c>
-      <c r="C76" t="s">
-        <v>8</v>
+      <c r="B76" s="3">
+        <v>2</v>
+      </c>
+      <c r="C76" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A77">
         <v>75</v>
       </c>
-      <c r="B77" t="s">
-        <v>3</v>
-      </c>
-      <c r="C77" t="s">
-        <v>6</v>
+      <c r="B77" s="3">
+        <v>1</v>
+      </c>
+      <c r="C77" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A78">
         <v>76</v>
       </c>
-      <c r="B78" t="s">
-        <v>3</v>
-      </c>
-      <c r="C78" t="s">
-        <v>8</v>
+      <c r="B78" s="3">
+        <v>1</v>
+      </c>
+      <c r="C78" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A79">
         <v>77</v>
       </c>
-      <c r="B79" t="s">
-        <v>4</v>
-      </c>
-      <c r="C79" t="s">
-        <v>6</v>
+      <c r="B79" s="3">
+        <v>2</v>
+      </c>
+      <c r="C79" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A80">
         <v>78</v>
       </c>
-      <c r="B80" t="s">
-        <v>3</v>
-      </c>
-      <c r="C80" t="s">
-        <v>8</v>
+      <c r="B80" s="3">
+        <v>1</v>
+      </c>
+      <c r="C80" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A81">
         <v>79</v>
       </c>
-      <c r="B81" t="s">
-        <v>3</v>
-      </c>
-      <c r="C81" t="s">
-        <v>7</v>
+      <c r="B81" s="3">
+        <v>1</v>
+      </c>
+      <c r="C81" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A82">
         <v>80</v>
       </c>
-      <c r="B82" t="s">
-        <v>5</v>
-      </c>
-      <c r="C82" t="s">
-        <v>6</v>
+      <c r="B82" s="3">
+        <v>3</v>
+      </c>
+      <c r="C82" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A83">
         <v>81</v>
       </c>
-      <c r="B83" t="s">
-        <v>5</v>
-      </c>
-      <c r="C83" t="s">
-        <v>6</v>
+      <c r="B83" s="3">
+        <v>3</v>
+      </c>
+      <c r="C83" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A84">
         <v>82</v>
       </c>
-      <c r="B84" t="s">
-        <v>3</v>
-      </c>
-      <c r="C84" t="s">
-        <v>8</v>
+      <c r="B84" s="3">
+        <v>1</v>
+      </c>
+      <c r="C84" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A85">
         <v>83</v>
       </c>
-      <c r="B85" t="s">
-        <v>5</v>
-      </c>
-      <c r="C85" t="s">
-        <v>8</v>
+      <c r="B85" s="3">
+        <v>3</v>
+      </c>
+      <c r="C85" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A86">
         <v>84</v>
       </c>
-      <c r="B86" t="s">
-        <v>5</v>
-      </c>
-      <c r="C86" t="s">
-        <v>8</v>
+      <c r="B86" s="3">
+        <v>3</v>
+      </c>
+      <c r="C86" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A87">
         <v>85</v>
       </c>
-      <c r="B87" t="s">
-        <v>3</v>
-      </c>
-      <c r="C87" t="s">
-        <v>6</v>
+      <c r="B87" s="3">
+        <v>1</v>
+      </c>
+      <c r="C87" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A88">
         <v>86</v>
       </c>
-      <c r="B88" t="s">
-        <v>3</v>
-      </c>
-      <c r="C88" t="s">
-        <v>8</v>
+      <c r="B88" s="3">
+        <v>1</v>
+      </c>
+      <c r="C88" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A89">
         <v>87</v>
       </c>
-      <c r="B89" t="s">
-        <v>3</v>
-      </c>
-      <c r="C89" t="s">
-        <v>7</v>
+      <c r="B89" s="3">
+        <v>1</v>
+      </c>
+      <c r="C89" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A90">
         <v>88</v>
       </c>
-      <c r="B90" t="s">
-        <v>3</v>
-      </c>
-      <c r="C90" t="s">
-        <v>7</v>
+      <c r="B90" s="3">
+        <v>1</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A91">
         <v>89</v>
       </c>
-      <c r="B91" t="s">
-        <v>3</v>
-      </c>
-      <c r="C91" t="s">
-        <v>8</v>
+      <c r="B91" s="3">
+        <v>1</v>
+      </c>
+      <c r="C91" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A92">
         <v>90</v>
       </c>
-      <c r="B92" t="s">
-        <v>3</v>
-      </c>
-      <c r="C92" t="s">
-        <v>7</v>
+      <c r="B92" s="3">
+        <v>1</v>
+      </c>
+      <c r="C92" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A93">
         <v>91</v>
       </c>
-      <c r="B93" t="s">
-        <v>4</v>
-      </c>
-      <c r="C93" t="s">
-        <v>6</v>
+      <c r="B93" s="3">
+        <v>2</v>
+      </c>
+      <c r="C93" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A94">
         <v>92</v>
       </c>
-      <c r="B94" t="s">
-        <v>3</v>
-      </c>
-      <c r="C94" t="s">
-        <v>6</v>
+      <c r="B94" s="3">
+        <v>1</v>
+      </c>
+      <c r="C94" s="3">
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A95">
         <v>93</v>
       </c>
-      <c r="B95" t="s">
-        <v>4</v>
-      </c>
-      <c r="C95" t="s">
-        <v>8</v>
+      <c r="B95" s="3">
+        <v>2</v>
+      </c>
+      <c r="C95" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96">
         <v>94</v>
       </c>
-      <c r="B96" t="s">
-        <v>4</v>
-      </c>
-      <c r="C96" t="s">
-        <v>8</v>
+      <c r="B96" s="3">
+        <v>2</v>
+      </c>
+      <c r="C96" s="3">
+        <v>1</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97">
         <v>95</v>
       </c>
-      <c r="B97" t="s">
-        <v>3</v>
-      </c>
-      <c r="C97" t="s">
-        <v>7</v>
+      <c r="B97" s="3">
+        <v>1</v>
+      </c>
+      <c r="C97" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A98">
         <v>96</v>
       </c>
-      <c r="B98" t="s">
-        <v>5</v>
-      </c>
-      <c r="C98" t="s">
-        <v>7</v>
+      <c r="B98" s="3">
+        <v>3</v>
+      </c>
+      <c r="C98" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99">
         <v>97</v>
       </c>
-      <c r="B99" t="s">
-        <v>4</v>
-      </c>
-      <c r="C99" t="s">
-        <v>7</v>
+      <c r="B99" s="3">
+        <v>2</v>
+      </c>
+      <c r="C99" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A100">
         <v>98</v>
       </c>
-      <c r="B100" t="s">
-        <v>4</v>
-      </c>
-      <c r="C100" t="s">
-        <v>7</v>
+      <c r="B100" s="3">
+        <v>2</v>
+      </c>
+      <c r="C100" s="3">
+        <v>2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A101">
         <v>99</v>
       </c>
-      <c r="B101" t="s">
-        <v>4</v>
-      </c>
-      <c r="C101" t="s">
-        <v>7</v>
+      <c r="B101" s="3">
+        <v>2</v>
+      </c>
+      <c r="C101" s="3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="C1:C101" xr:uid="{58BEDD75-86AB-E343-9D27-EC784ACDACA4}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>